<commit_message>
Working on lit search
</commit_message>
<xml_diff>
--- a/NCC_conceptual_paper/study summary.xlsx
+++ b/NCC_conceptual_paper/study summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="33340" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="25600" yWindow="5600" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="all studies" sheetId="4" r:id="rId1"/>
@@ -4563,7 +4563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
@@ -5647,13 +5647,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5713,66 +5713,57 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>270</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>42</v>
+        <v>266</v>
       </c>
       <c r="H2" s="32" t="s">
-        <v>42</v>
+        <v>268</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="4">
-        <v>1</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>44</v>
+        <v>267</v>
       </c>
       <c r="L2" s="4"/>
-      <c r="M2" s="4" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
-        <v>273</v>
+        <v>58</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>274</v>
+        <v>285</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
       <c r="H3" s="32" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>50</v>
+        <v>185</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4" t="s">
@@ -5781,593 +5772,575 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>48</v>
+        <v>176</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>186</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>62</v>
+        <v>182</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>62</v>
+        <v>183</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>53</v>
+        <v>181</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" s="4">
-        <v>1</v>
-      </c>
-      <c r="K4" s="4">
-        <v>1</v>
-      </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4" t="s">
-        <v>43</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
-        <v>284</v>
+        <v>58</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="32" t="s">
-        <v>42</v>
+        <v>176</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>178</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4" t="s">
-        <v>43</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1"/>
+      <c r="A6" s="4" t="s">
+        <v>394</v>
+      </c>
       <c r="C6" s="4" t="s">
-        <v>58</v>
+        <v>390</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>285</v>
+        <v>383</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>63</v>
+        <v>265</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="H6" s="32" t="s">
-        <v>60</v>
+        <v>253</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>393</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="J6" s="4">
-        <v>1</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>61</v>
+        <v>253</v>
       </c>
       <c r="L6" s="4"/>
-      <c r="M6" s="4" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>256</v>
+      </c>
       <c r="C7" s="4" t="s">
-        <v>48</v>
+        <v>140</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>287</v>
+        <v>144</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>288</v>
+        <v>146</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>290</v>
+        <v>142</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>289</v>
+        <v>142</v>
       </c>
       <c r="H7" s="32" t="s">
-        <v>291</v>
+        <v>67</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="J7" s="4">
-        <v>1</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="L7" s="4"/>
+        <v>143</v>
+      </c>
       <c r="M7" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="H8" s="32" t="s">
-        <v>162</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="L8" s="4"/>
+      <c r="A8" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="27" t="s">
+        <v>254</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="H8" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="27" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="H9" s="32" t="s">
-        <v>268</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="L9" s="4"/>
+      <c r="C9" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="J9" s="6">
+        <v>1</v>
+      </c>
+      <c r="K9" s="6"/>
+      <c r="M9" s="6" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
-        <v>69</v>
+        <v>247</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>70</v>
+        <v>248</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>117</v>
+        <v>249</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>72</v>
+        <v>148</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>250</v>
       </c>
       <c r="H10" s="32" t="s">
-        <v>74</v>
+        <v>252</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4" t="s">
-        <v>43</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="1"/>
+      <c r="A11" s="4" t="s">
+        <v>426</v>
+      </c>
       <c r="C11" s="4" t="s">
-        <v>69</v>
+        <v>302</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>70</v>
+        <v>430</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>117</v>
+        <v>429</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="H11" s="32" t="s">
-        <v>74</v>
+        <v>265</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>431</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>54</v>
+        <v>185</v>
       </c>
       <c r="L11" s="4"/>
-      <c r="M11" s="4" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1"/>
+      <c r="A12" s="4" t="s">
+        <v>441</v>
+      </c>
       <c r="C12" s="4" t="s">
-        <v>69</v>
+        <v>302</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>70</v>
+        <v>428</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>92</v>
+        <v>444</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>265</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="H12" s="32" t="s">
-        <v>94</v>
+        <v>445</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>440</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>54</v>
+        <v>253</v>
       </c>
       <c r="L12" s="4"/>
-      <c r="M12" s="4" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="1"/>
+      <c r="A13" s="4" t="s">
+        <v>409</v>
+      </c>
       <c r="C13" s="4" t="s">
-        <v>69</v>
+        <v>302</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>230</v>
+        <v>403</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>405</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="H13" s="32" t="s">
-        <v>232</v>
+        <v>142</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>406</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>54</v>
+        <v>253</v>
       </c>
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="4" t="s">
-        <v>236</v>
+      <c r="A14" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>302</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>239</v>
+        <v>383</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>385</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="H14" s="32" t="s">
-        <v>240</v>
+        <v>253</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>382</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>214</v>
+        <v>253</v>
       </c>
       <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="1"/>
+      <c r="A15" s="4" t="s">
+        <v>446</v>
+      </c>
       <c r="C15" s="4" t="s">
-        <v>69</v>
+        <v>302</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>230</v>
+        <v>383</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>447</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="H15" s="32" t="s">
-        <v>232</v>
+        <v>344</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>449</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>54</v>
+        <v>451</v>
       </c>
       <c r="L15" s="4"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="1"/>
+      <c r="A16" s="4" t="s">
+        <v>168</v>
+      </c>
       <c r="C16" s="4" t="s">
-        <v>222</v>
+        <v>302</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>223</v>
+        <v>176</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>309</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>226</v>
+        <v>311</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="H16" s="32" t="s">
-        <v>227</v>
+        <v>185</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>312</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>228</v>
+        <v>185</v>
       </c>
       <c r="L16" s="4"/>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="1"/>
+      <c r="A17" s="4" t="s">
+        <v>169</v>
+      </c>
       <c r="C17" s="4" t="s">
-        <v>216</v>
+        <v>302</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>217</v>
+        <v>176</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>315</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>153</v>
+        <v>182</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="H17" s="32" t="s">
-        <v>162</v>
+        <v>185</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>316</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>219</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="L17" s="4"/>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="1"/>
+      <c r="A18" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="C18" s="4" t="s">
-        <v>207</v>
+        <v>302</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>208</v>
+        <v>304</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>303</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>209</v>
+        <v>305</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="H18" s="32" t="s">
-        <v>213</v>
+        <v>297</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>306</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>214</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="L18" s="4"/>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>197</v>
+      <c r="A19" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>328</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="H19" s="32" t="s">
-        <v>162</v>
+        <v>185</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>329</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>162</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="L19" s="4"/>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="5"/>
+      <c r="A20" s="4" t="s">
+        <v>335</v>
+      </c>
       <c r="C20" s="4" t="s">
-        <v>190</v>
+        <v>302</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>54</v>
+        <v>248</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>192</v>
+        <v>265</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="H20" s="32" t="s">
-        <v>195</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>196</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="L20" s="4"/>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="1"/>
+      <c r="A21" s="4" t="s">
+        <v>436</v>
+      </c>
       <c r="C21" s="4" t="s">
-        <v>58</v>
+        <v>302</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>186</v>
+        <v>439</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>182</v>
+        <v>265</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="H21" s="32" t="s">
-        <v>181</v>
+        <v>185</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>440</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>185</v>
       </c>
+      <c r="L21" s="4"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="1"/>
+      <c r="A22" s="4" t="s">
+        <v>348</v>
+      </c>
       <c r="C22" s="4" t="s">
-        <v>58</v>
+        <v>302</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="H22" s="31" t="s">
-        <v>178</v>
+        <v>352</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>355</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>185</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="L22" s="4"/>
     </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="H23" s="32" t="s">
-        <v>162</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="M23" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>277</v>
+        <v>157</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="H24" s="31" t="s">
-        <v>153</v>
-      </c>
-      <c r="I24" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="H24" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="I24" s="4" t="s">
         <v>162</v>
       </c>
       <c r="M24" s="4" t="s">
@@ -6375,711 +6348,760 @@
       </c>
     </row>
     <row r="25" spans="1:13" s="27" customFormat="1" ht="55" customHeight="1">
-      <c r="A25" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="26"/>
-      <c r="C25" s="27" t="s">
-        <v>254</v>
-      </c>
-      <c r="D25" s="27" t="s">
-        <v>248</v>
-      </c>
-      <c r="E25" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="F25" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="G25" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="H25" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="I25" s="29" t="s">
-        <v>253</v>
-      </c>
-      <c r="L25" s="30"/>
-      <c r="M25" s="27" t="s">
+      <c r="A25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H25" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J25" s="4">
+        <v>1</v>
+      </c>
+      <c r="K25" s="4">
+        <v>1</v>
+      </c>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="4" t="s">
-        <v>247</v>
+        <v>48</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>248</v>
+        <v>277</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="H26" s="32" t="s">
-        <v>252</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>185</v>
+        <v>154</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="H26" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>138</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B27" s="1"/>
       <c r="C27" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>279</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="G27" s="35" t="s">
-        <v>280</v>
+        <v>48</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="H27" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="I27" s="16" t="s">
-        <v>135</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J27" s="4">
+        <v>1</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L27" s="4"/>
       <c r="M27" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>124</v>
+        <v>15</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>132</v>
+        <v>287</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F28" s="35" t="s">
-        <v>280</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="H28" s="36" t="s">
-        <v>135</v>
+        <v>288</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="H28" s="32" t="s">
+        <v>291</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>185</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="J28" s="4">
+        <v>1</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="L28" s="4"/>
       <c r="M28" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:13">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="L29" s="4"/>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="9"/>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="E31" s="37" t="s">
+        <v>294</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="L31" s="4"/>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="H32" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="H33" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="H34" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="H35" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="H36" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G37" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="H37" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="I37" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H38" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H39" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="L39" s="4"/>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="H40" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="H41" s="32" t="s">
+        <v>240</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L41" s="4"/>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="H42" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="L42" s="4"/>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="4" t="s">
+      <c r="B43" s="1"/>
+      <c r="C43" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E43" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F43" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G43" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="H29" s="32" t="s">
+      <c r="H43" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="I29" s="6" t="s">
+      <c r="I43" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="M29" s="4" t="s">
+      <c r="M43" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="1" t="s">
+    <row r="44" spans="1:13">
+      <c r="A44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H44" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H45" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H46" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="4" t="s">
+      <c r="B47" s="1"/>
+      <c r="C47" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D47" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E47" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F47" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="G47" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="H30" s="32" t="s">
+      <c r="H47" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="I30" s="6" t="s">
+      <c r="I47" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="M30" s="4" t="s">
+      <c r="M47" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="H31" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="J31" s="6">
-        <v>1</v>
-      </c>
-      <c r="K31" s="6"/>
-      <c r="M31" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="E32" s="37" t="s">
-        <v>294</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="L32" s="4"/>
-    </row>
-    <row r="33" spans="1:9" s="4" customFormat="1">
-      <c r="A33" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="4" customFormat="1">
-      <c r="A34" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" s="4" customFormat="1">
-      <c r="A35" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="4" customFormat="1">
-      <c r="A36" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="4" customFormat="1">
-      <c r="A37" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="4" customFormat="1">
-      <c r="A38" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="4" customFormat="1">
-      <c r="A39" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="4" customFormat="1">
-      <c r="A40" s="4" t="s">
+    <row r="48" spans="1:13">
+      <c r="A48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H48" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L48" s="4"/>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H49" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L49" s="4"/>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" s="4" t="s">
         <v>324</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>302</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="F40" s="16" t="s">
-        <v>385</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="H40" s="16" t="s">
-        <v>382</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" s="4" customFormat="1">
-      <c r="A41" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>390</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>393</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" s="4" customFormat="1">
-      <c r="A42" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>398</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>399</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>400</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>401</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="4" customFormat="1">
-      <c r="A43" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>403</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>405</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="4" customFormat="1">
-      <c r="A44" s="4" t="s">
-        <v>426</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>429</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>431</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" s="4" customFormat="1">
-      <c r="A45" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>439</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>440</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" s="4" customFormat="1">
-      <c r="A46" s="4" t="s">
-        <v>441</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>428</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>444</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>440</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" s="4" customFormat="1">
-      <c r="A47" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>447</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>450</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>449</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13">
-      <c r="A49" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F49" s="9"/>
-      <c r="G49" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="9"/>
-    </row>
-    <row r="50" spans="1:13">
-      <c r="A50" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>256</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>146</v>
+        <v>379</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>302</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="H50" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="I50" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="M50" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13">
-      <c r="A51" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="D51" s="16" t="s">
-        <v>302</v>
-      </c>
-      <c r="F51" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="G51" s="16" t="s">
+      <c r="G50" s="16" t="s">
         <v>381</v>
       </c>
-      <c r="H51" s="4" t="s">
+      <c r="H50" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="I51" s="16" t="s">
+      <c r="I50" s="16" t="s">
         <v>382</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:M51">
+    <sortCondition ref="C2:C51"/>
+    <sortCondition ref="D2:D51"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>